<commit_message>
fix(general): fix bug date
</commit_message>
<xml_diff>
--- a/src/modules/voucher/public/voucher_date-514a1d0c-d201-4e16-a221-9359779481ee.xlsx
+++ b/src/modules/voucher/public/voucher_date-514a1d0c-d201-4e16-a221-9359779481ee.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
   <si>
     <t>code</t>
   </si>
@@ -43,25 +43,55 @@
     <t>createdAt</t>
   </si>
   <si>
+    <t>I0GOTQFEZC9FWW3Y</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>ONLINE</t>
+  </si>
+  <si>
+    <t>COUPON</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>11/09/2022</t>
+  </si>
+  <si>
+    <t>29/09/2022</t>
+  </si>
+  <si>
+    <t>10/09/2022</t>
+  </si>
+  <si>
+    <t>C63OACLO0NLWS0N0</t>
+  </si>
+  <si>
+    <t>56ZMXEMC13RMC380</t>
+  </si>
+  <si>
+    <t>07/09/2022</t>
+  </si>
+  <si>
+    <t>30/09/2022</t>
+  </si>
+  <si>
+    <t>AA33C0AJ336BJQA0</t>
+  </si>
+  <si>
+    <t>AAS3DWWRVOFC52TW</t>
+  </si>
+  <si>
+    <t>9HIHJDIPM50AC6NA</t>
+  </si>
+  <si>
     <t>AF06WSE3TAJCAPQB</t>
   </si>
   <si>
-    <t>ACTIVE</t>
-  </si>
-  <si>
-    <t>ONLINE</t>
-  </si>
-  <si>
-    <t>COUPON</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>05/09/2022</t>
-  </si>
-  <si>
-    <t>30/09/2022</t>
   </si>
   <si>
     <t>8IHBFU05FZAE9QEC</t>
@@ -468,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="40" style="1" customWidth="1"/>
@@ -525,7 +555,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>14</v>
@@ -538,12 +568,12 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -555,7 +585,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
@@ -568,12 +598,12 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -585,25 +615,25 @@
         <v>13</v>
       </c>
       <c r="E4" s="1">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -615,76 +645,256 @@
         <v>13</v>
       </c>
       <c r="E5" s="1">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2">
-        <v>56</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2">
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1">
         <v>56</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>15</v>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1">
+        <v>56</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
+        <v>56</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2">
+        <v>56</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2">
+        <v>56</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>